<commit_message>
Complex parameterization with Hashtables
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>TestCases</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Vasya Vasiliev</t>
+  </si>
+  <si>
+    <t>Test Testov</t>
+  </si>
+  <si>
+    <t>Kalim Neon</t>
   </si>
 </sst>
 </file>
@@ -456,10 +462,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -560,6 +566,28 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>